<commit_message>
Nuevos datos actualizados con API
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B450A23-B807-4E79-AF1E-B85A4A5FC482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDC7AED-2405-4C0F-9152-56BE1819FA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A6148338-BA43-4A68-9E5E-C6F26008496C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
   <si>
     <t>USUARIO</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>idComentario, idReportante</t>
+  </si>
+  <si>
+    <t>obtenerUsuarioPorUsername</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -363,7 +369,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,15 +706,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382BC564-540B-47B1-8FA3-4484D8E47885}">
-  <dimension ref="A2:G76"/>
+  <dimension ref="A2:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="2" max="2" width="40.88671875" customWidth="1"/>
     <col min="6" max="6" width="35.6640625" customWidth="1"/>
     <col min="7" max="7" width="47.21875" customWidth="1"/>
@@ -727,14 +735,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="B3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -764,644 +772,634 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="B13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="F18" s="4" t="s">
+      <c r="B19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="F22" s="3" t="s">
+      <c r="B23" s="4"/>
+      <c r="F23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="F28" s="3" t="s">
+      <c r="B29" s="4"/>
+      <c r="F29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>75</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="F45" s="4" t="s">
+      <c r="B46" s="4"/>
+      <c r="F46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G46" t="s">
-        <v>64</v>
-      </c>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G49" s="4"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G50" t="s">
-        <v>66</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="G51" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>10</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="F54" s="4" t="s">
+      <c r="B55" s="4"/>
+      <c r="F55" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G54" s="4"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" t="s">
-        <v>38</v>
-      </c>
-      <c r="G55" t="s">
-        <v>59</v>
-      </c>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G56" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" t="s">
+        <v>40</v>
+      </c>
+      <c r="G58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>16</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>52</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>41</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="F60" s="4" t="s">
+      <c r="B61" s="4"/>
+      <c r="F61" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G60" s="4"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" t="s">
-        <v>43</v>
-      </c>
+      <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>19</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>55</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F63" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B64" s="4"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" t="s">
-        <v>52</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
-      </c>
-      <c r="F66" t="s">
-        <v>47</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G66" s="4"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F67" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>23</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>58</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F69" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B70" s="4"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>26</v>
-      </c>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>29</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="A64:B64"/>
+  <mergeCells count="3">
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Paso de objeto, convertido a json y leido por kotlin
</commit_message>
<xml_diff>
--- a/Organizacion.xlsx
+++ b/Organizacion.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDC7AED-2405-4C0F-9152-56BE1819FA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A78103E-F988-4A59-B240-3545E7B28671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A6148338-BA43-4A68-9E5E-C6F26008496C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{A6148338-BA43-4A68-9E5E-C6F26008496C}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
+    <sheet name="Movil" sheetId="2" r:id="rId2"/>
+    <sheet name="Escritorio" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="98">
   <si>
     <t>USUARIO</t>
   </si>
@@ -297,13 +299,46 @@
   </si>
   <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>APLICACIÓN DE ESCRITORIO</t>
+  </si>
+  <si>
+    <t>PARTE VISUAL</t>
+  </si>
+  <si>
+    <t>MDI</t>
+  </si>
+  <si>
+    <t>Lista Principal</t>
+  </si>
+  <si>
+    <t>Informacion usuarios - Admi</t>
+  </si>
+  <si>
+    <t>Informacion usuarios - Normal</t>
+  </si>
+  <si>
+    <t>Info Libro</t>
+  </si>
+  <si>
+    <t>Lista Libros Erroneos</t>
+  </si>
+  <si>
+    <t>Lista comentarios Reportados</t>
+  </si>
+  <si>
+    <t>Info comentario</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN BASICA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +346,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +386,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -356,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,6 +433,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382BC564-540B-47B1-8FA3-4484D8E47885}">
   <dimension ref="A2:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1403,4 +1474,141 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5929A77-BA9C-4A58-AD53-5DB2456EEE6C}">
+  <dimension ref="A2:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="D2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225061A8-D339-40B3-BE7E-1C2F2671ECA1}">
+  <dimension ref="A2:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>